<commit_message>
additional information in database design
as per summary
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.alpha.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.alpha.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="233">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -83,24 +83,6 @@
     <t>customer_email</t>
   </si>
   <si>
-    <t>GROUP CUSTOMER</t>
-  </si>
-  <si>
-    <t>group_customer_id</t>
-  </si>
-  <si>
-    <t>group_customer_name</t>
-  </si>
-  <si>
-    <t>group_customer_discount</t>
-  </si>
-  <si>
-    <t>customer_level_joined_date</t>
-  </si>
-  <si>
-    <t>customer_level_total_sales_count</t>
-  </si>
-  <si>
     <t>SUPPLIER</t>
   </si>
   <si>
@@ -233,33 +215,15 @@
     <t>1,2,3,4,5,6</t>
   </si>
   <si>
-    <t>default new customer group is grosir</t>
-  </si>
-  <si>
     <t>PRODUCTS</t>
   </si>
   <si>
-    <t>MASTER PRODUCTS</t>
-  </si>
-  <si>
     <t>user_name</t>
   </si>
   <si>
     <t>module_active</t>
   </si>
   <si>
-    <t>MASTER RANK</t>
-  </si>
-  <si>
-    <t>rank_id</t>
-  </si>
-  <si>
-    <t>rank_name</t>
-  </si>
-  <si>
-    <t>user_rank_id</t>
-  </si>
-  <si>
     <t>unique</t>
   </si>
   <si>
@@ -278,9 +242,6 @@
     <t>user_active</t>
   </si>
   <si>
-    <t>rank_active</t>
-  </si>
-  <si>
     <t>group_user_active</t>
   </si>
   <si>
@@ -293,9 +254,6 @@
     <t>customer_active</t>
   </si>
   <si>
-    <t>group_customer_active</t>
-  </si>
-  <si>
     <t>supplier_active</t>
   </si>
   <si>
@@ -320,51 +278,15 @@
     <t>products_id</t>
   </si>
   <si>
-    <t>products_name</t>
-  </si>
-  <si>
-    <t>pembulatan ke atas terdekat 100</t>
-  </si>
-  <si>
     <t>harga beli</t>
   </si>
   <si>
-    <t>products_description</t>
-  </si>
-  <si>
     <t>products_base_price</t>
   </si>
   <si>
-    <t>products_margin_percentage</t>
-  </si>
-  <si>
     <t>products_sales_price</t>
   </si>
   <si>
-    <t>products_photo_1</t>
-  </si>
-  <si>
-    <t>products_photo_2</t>
-  </si>
-  <si>
-    <t>products_photo_3</t>
-  </si>
-  <si>
-    <t>products_photo_4</t>
-  </si>
-  <si>
-    <t>products_photo_5</t>
-  </si>
-  <si>
-    <t>products_stock</t>
-  </si>
-  <si>
-    <t>products_limit_stock</t>
-  </si>
-  <si>
-    <t>GROUP CUSTOMER DISCOUNT</t>
-  </si>
-  <si>
     <t>product_id</t>
   </si>
   <si>
@@ -377,9 +299,6 @@
     <t>tags_desctiption</t>
   </si>
   <si>
-    <t>products_active</t>
-  </si>
-  <si>
     <t>unit_active</t>
   </si>
   <si>
@@ -392,9 +311,6 @@
     <t>1=sales, 2=mutasi, 3=adjustment</t>
   </si>
   <si>
-    <t>products_shelves</t>
-  </si>
-  <si>
     <t>BRANCH MANAGEMENT</t>
   </si>
   <si>
@@ -461,18 +377,9 @@
     <t>products_price</t>
   </si>
   <si>
-    <t>products_unit</t>
-  </si>
-  <si>
-    <t>purchase_top</t>
-  </si>
-  <si>
     <t>purchase_paid</t>
   </si>
   <si>
-    <t>purchase_top_date</t>
-  </si>
-  <si>
     <t>DEBT</t>
   </si>
   <si>
@@ -575,9 +482,6 @@
     <t>sales_discount_final</t>
   </si>
   <si>
-    <t>sales_discount_customer</t>
-  </si>
-  <si>
     <t>sales_top</t>
   </si>
   <si>
@@ -620,9 +524,6 @@
     <t>rp_processed</t>
   </si>
   <si>
-    <t>rs_processed</t>
-  </si>
-  <si>
     <t>debt_datetime</t>
   </si>
   <si>
@@ -669,22 +570,158 @@
   </si>
   <si>
     <t>login,logout,insert,update,delete,view,active,open cashier, close cashier</t>
+  </si>
+  <si>
+    <t>change_ip</t>
+  </si>
+  <si>
+    <t>change_shift</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>CUSTOMER SALES HISTORY</t>
+  </si>
+  <si>
+    <t>discount_1</t>
+  </si>
+  <si>
+    <t>discount_2</t>
+  </si>
+  <si>
+    <t>discount_rp</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>customer_joined_date</t>
+  </si>
+  <si>
+    <t>customer_total_sales_count</t>
+  </si>
+  <si>
+    <t>ecer, grosir, partai</t>
+  </si>
+  <si>
+    <t>customer_group</t>
+  </si>
+  <si>
+    <t>product_name</t>
+  </si>
+  <si>
+    <t>product_description</t>
+  </si>
+  <si>
+    <t>product_base_price</t>
+  </si>
+  <si>
+    <t>product_retail_price</t>
+  </si>
+  <si>
+    <t>product_bulk_price</t>
+  </si>
+  <si>
+    <t>product_wholesale_price</t>
+  </si>
+  <si>
+    <t>product_photo_1</t>
+  </si>
+  <si>
+    <t>product_photo_2</t>
+  </si>
+  <si>
+    <t>product_photo_3</t>
+  </si>
+  <si>
+    <t>product_photo_4</t>
+  </si>
+  <si>
+    <t>product_photo_5</t>
+  </si>
+  <si>
+    <t>product_stock_qty</t>
+  </si>
+  <si>
+    <t>product_limit_stock</t>
+  </si>
+  <si>
+    <t>product_shelves</t>
+  </si>
+  <si>
+    <t>product_active</t>
+  </si>
+  <si>
+    <t>MASTER PRODUCT</t>
+  </si>
+  <si>
+    <t>product_brand</t>
+  </si>
+  <si>
+    <t>temp not use</t>
+  </si>
+  <si>
+    <t>bisa desimal 2 digit</t>
+  </si>
+  <si>
+    <t>PRODUCT LOSS</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>new_product_id</t>
+  </si>
+  <si>
+    <t>new_qty</t>
+  </si>
+  <si>
+    <t>total_loss</t>
+  </si>
+  <si>
+    <t>product_is_service</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>purchase_term_of_payment</t>
+  </si>
+  <si>
+    <t>purchase_term_of_payment_date</t>
+  </si>
+  <si>
+    <t>product_disc_1</t>
+  </si>
+  <si>
+    <t>product_disc_2</t>
+  </si>
+  <si>
+    <t>product_disc_rp</t>
+  </si>
+  <si>
+    <t>sales_subtotal</t>
+  </si>
+  <si>
+    <t>RETURN SALES HEADER STOCK ADJUSTMENT</t>
+  </si>
+  <si>
+    <t>RETURN SALES DETAIL STOCK ADJUSTMENT</t>
+  </si>
+  <si>
+    <t>DATABASE_NAME = SYS_POS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -712,12 +749,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,7 +818,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -813,7 +853,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1022,20 +1062,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q229"/>
+  <dimension ref="B1:Q246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="C260" sqref="C260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>232</v>
+      </c>
+    </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
@@ -1049,13 +1095,13 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1066,70 +1112,70 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -1145,18 +1191,18 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
@@ -1166,1178 +1212,1253 @@
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>64</v>
+        <v>74</v>
+      </c>
+      <c r="F21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" t="s">
+        <v>72</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="P21" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>86</v>
-      </c>
-      <c r="F22" t="s">
-        <v>68</v>
-      </c>
-      <c r="H22" t="s">
-        <v>84</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="P22" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>54</v>
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
       <c r="D23" t="s">
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>59</v>
+      </c>
+      <c r="N23" t="s">
+        <v>47</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>77</v>
-      </c>
       <c r="D24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" t="s">
-        <v>67</v>
+        <v>76</v>
+      </c>
+      <c r="N24" t="s">
+        <v>48</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+      <c r="Q24">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="N25" t="s">
+        <v>49</v>
+      </c>
+      <c r="P25">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="N27" t="s">
-        <v>53</v>
-      </c>
-      <c r="P27">
-        <v>1</v>
-      </c>
-      <c r="Q27">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>89</v>
-      </c>
-      <c r="N28" t="s">
-        <v>54</v>
-      </c>
-      <c r="P28">
-        <v>2</v>
-      </c>
-      <c r="Q28">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>90</v>
-      </c>
-      <c r="N29" t="s">
-        <v>55</v>
-      </c>
-      <c r="P29">
-        <v>3</v>
+        <v>64</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
       <c r="D30" t="s">
-        <v>88</v>
-      </c>
-      <c r="F30" t="s">
-        <v>68</v>
-      </c>
-      <c r="H30" t="s">
-        <v>84</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>9</v>
-      </c>
       <c r="D31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" t="s">
-        <v>5</v>
-      </c>
-      <c r="N31" t="s">
-        <v>56</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" t="s">
-        <v>5</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>96</v>
-      </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" s="1"/>
+        <v>186</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>182</v>
+      </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="E38" s="1"/>
+      <c r="H38" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>215</v>
-      </c>
-      <c r="D39" t="s">
-        <v>2</v>
-      </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>216</v>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="H40" t="s">
-        <v>217</v>
+      <c r="B40" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E41" s="1"/>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>14</v>
+      <c r="D42" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>15</v>
-      </c>
       <c r="D43" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>21</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>91</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>27</v>
+        <v>197</v>
+      </c>
+      <c r="H50" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>188</v>
+      </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>22</v>
-      </c>
       <c r="D53" t="s">
-        <v>23</v>
-      </c>
-      <c r="E53" t="s">
-        <v>65</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>92</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>115</v>
-      </c>
       <c r="D56" t="s">
-        <v>116</v>
+        <v>190</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>23</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>25</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D61" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E61" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G61" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>93</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>73</v>
+      <c r="C70" t="s">
+        <v>213</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>74</v>
-      </c>
       <c r="D71" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="E71" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E72" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>94</v>
-      </c>
-      <c r="E73" t="s">
-        <v>81</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>104</v>
+        <v>200</v>
+      </c>
+      <c r="G75" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>105</v>
-      </c>
-      <c r="G76" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>106</v>
-      </c>
-      <c r="G77" t="s">
-        <v>102</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>107</v>
+        <v>203</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>108</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D84" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E84" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E85" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="E86" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>222</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="93" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
+      <c r="D93" t="s">
+        <v>2</v>
+      </c>
+      <c r="E93" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>86</v>
+      </c>
+      <c r="E94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="96" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>34</v>
+      </c>
+      <c r="F97" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>217</v>
+      </c>
+      <c r="D99" t="s">
+        <v>2</v>
+      </c>
+      <c r="E99" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="107" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>35</v>
+      </c>
+      <c r="D107" t="s">
+        <v>31</v>
+      </c>
+      <c r="E107" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="109" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="110" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="112" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>36</v>
+      </c>
+      <c r="D112" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>40</v>
+      </c>
+      <c r="D116" t="s">
+        <v>30</v>
+      </c>
+      <c r="E116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="119" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="121" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>44</v>
+      </c>
+      <c r="D121" t="s">
+        <v>2</v>
+      </c>
+      <c r="E121" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D122" t="s">
+        <v>96</v>
+      </c>
+      <c r="E122" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="125" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="126" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="127" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="128" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>156</v>
-      </c>
-      <c r="D91" t="s">
-        <v>2</v>
-      </c>
-      <c r="E91" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D92" t="s">
-        <v>100</v>
-      </c>
-      <c r="E92" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D93" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="94" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D94" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D95" t="s">
-        <v>40</v>
-      </c>
-      <c r="F95" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
-        <v>41</v>
-      </c>
-      <c r="D97" t="s">
-        <v>37</v>
-      </c>
-      <c r="E97" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D99" t="s">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
+        <v>43</v>
+      </c>
+      <c r="D130" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D100" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
-        <v>42</v>
-      </c>
-      <c r="D102" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D103" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="106" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C106" t="s">
-        <v>46</v>
-      </c>
-      <c r="D106" t="s">
-        <v>36</v>
-      </c>
-      <c r="E106" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="107" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D107" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="108" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D108" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="109" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D109" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C111" t="s">
-        <v>50</v>
-      </c>
-      <c r="D111" t="s">
-        <v>2</v>
-      </c>
-      <c r="E111" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D112" t="s">
-        <v>123</v>
-      </c>
-      <c r="E112" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D113" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D114" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D115" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D116" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D117" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D118" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C120" t="s">
-        <v>49</v>
-      </c>
-      <c r="D120" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D121" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D122" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D123" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D124" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D125" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C127" t="s">
-        <v>137</v>
-      </c>
-      <c r="D127" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D128" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D129" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D130" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="131" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
     </row>
     <row r="132" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
     </row>
     <row r="133" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="134" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D134" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
     </row>
     <row r="136" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="D136" t="s">
-        <v>154</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="138" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
     </row>
     <row r="139" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="140" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
     </row>
     <row r="141" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
     </row>
     <row r="142" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C144" t="s">
-        <v>167</v>
-      </c>
-      <c r="D144" t="s">
-        <v>2</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="145" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
+        <v>115</v>
+      </c>
       <c r="D145" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
     </row>
     <row r="146" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D146" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
     </row>
     <row r="147" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
     </row>
     <row r="148" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
-        <v>160</v>
+        <v>89</v>
       </c>
     </row>
     <row r="149" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C151" t="s">
-        <v>168</v>
-      </c>
-      <c r="D151" t="s">
-        <v>164</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="152" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
+        <v>136</v>
+      </c>
       <c r="D152" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
     </row>
     <row r="154" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
     </row>
     <row r="155" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
     </row>
     <row r="156" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
     </row>
     <row r="157" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="159" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C159" t="s">
-        <v>180</v>
+        <v>137</v>
       </c>
       <c r="D159" t="s">
-        <v>2</v>
+        <v>133</v>
       </c>
     </row>
     <row r="160" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D160" t="s">
-        <v>182</v>
+        <v>86</v>
       </c>
     </row>
     <row r="161" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D161" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
     </row>
     <row r="162" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
     </row>
     <row r="163" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
     </row>
     <row r="164" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D165" t="s">
-        <v>187</v>
+        <v>134</v>
       </c>
     </row>
     <row r="166" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C166" t="s">
+        <v>149</v>
+      </c>
       <c r="D166" t="s">
-        <v>188</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
-        <v>189</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D168" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C169" t="s">
-        <v>181</v>
-      </c>
       <c r="D169" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
     </row>
     <row r="170" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D170" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
     </row>
     <row r="171" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
     </row>
     <row r="172" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D172" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
     </row>
     <row r="173" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D173" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="174" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D174" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D175" t="s">
-        <v>52</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C176" t="s">
+        <v>150</v>
+      </c>
+      <c r="D176" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="177" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C177" t="s">
-        <v>169</v>
-      </c>
       <c r="D177" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
     </row>
     <row r="178" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D178" t="s">
-        <v>171</v>
+        <v>89</v>
       </c>
     </row>
     <row r="179" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D179" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
     </row>
     <row r="180" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
-        <v>173</v>
+        <v>229</v>
       </c>
     </row>
     <row r="181" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
-        <v>174</v>
+        <v>226</v>
       </c>
     </row>
     <row r="182" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D182" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="184" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C184" t="s">
-        <v>170</v>
-      </c>
-      <c r="D184" t="s">
-        <v>175</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="183" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D183" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="185" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C185" t="s">
+        <v>138</v>
+      </c>
       <c r="D185" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D186" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
     </row>
     <row r="187" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="188" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="189" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D189" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="190" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D190" t="s">
-        <v>177</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="191" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C191" t="s">
+        <v>139</v>
+      </c>
+      <c r="D191" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="192" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C192" t="s">
-        <v>191</v>
-      </c>
       <c r="D192" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="193" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D193" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="194" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D194" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="195" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D195" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="196" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D196" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="198" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C198" t="s">
+        <v>230</v>
+      </c>
+      <c r="D198" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D193" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D194" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D195" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D196" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D197" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C199" t="s">
-        <v>192</v>
-      </c>
+    <row r="199" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D199" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="200" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="201" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D202" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="203" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C203" t="s">
+        <v>231</v>
+      </c>
       <c r="D203" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="204" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D204" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B206" t="s">
-        <v>133</v>
-      </c>
-      <c r="C206" t="s">
-        <v>134</v>
-      </c>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="205" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D205" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="206" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D206" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="207" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D207" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="208" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D208" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="210" spans="3:4" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C210" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D210" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D211" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="212" spans="3:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D212" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="213" spans="3:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D213" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="214" spans="3:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D214" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="216" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C216" t="s">
-        <v>153</v>
-      </c>
-      <c r="D216" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D215" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C217" t="s">
+        <v>160</v>
+      </c>
+      <c r="D217" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D218" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D219" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D220" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D221" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
+        <v>105</v>
+      </c>
+      <c r="C223" t="s">
+        <v>106</v>
+      </c>
+      <c r="D223" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D217" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="218" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D218" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="219" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D219" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="220" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D220" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="222" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C222" t="s">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D224" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="225" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D225" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="227" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C227" t="s">
+        <v>121</v>
+      </c>
+      <c r="D227" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D228" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="229" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D229" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="230" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D230" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="231" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D231" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="233" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C233" t="s">
+        <v>122</v>
+      </c>
+      <c r="D233" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D234" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="235" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D235" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="236" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D236" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="237" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D237" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="239" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C239" t="s">
+        <v>147</v>
+      </c>
+      <c r="D239" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D240" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D241" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D242" t="s">
         <v>178</v>
       </c>
-      <c r="D222" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="223" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D223" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="224" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D224" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D225" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D226" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D227" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B229" t="s">
-        <v>214</v>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D243" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D244" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B246" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E80:E83"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2355,21 +2476,21 @@
   <sheetData>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2383,7 +2504,7 @@
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E11">
         <v>0</v>

</xml_diff>

<commit_message>
Add Code for Database Connection
Added Data_Access Module for database connection
Fix interface in dataPelangganDetail
Fix interface in dataProdukDetail
Fix interface in stokPecahBarang
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.alpha.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.alpha.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="234">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -714,6 +714,9 @@
   </si>
   <si>
     <t>DATABASE_NAME = SYS_POS</t>
+  </si>
+  <si>
+    <t>user_password</t>
   </si>
 </sst>
 </file>
@@ -754,10 +757,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q246"/>
+  <dimension ref="B1:Q247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="C260" sqref="C260"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,462 +1210,459 @@
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>3</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" t="s">
-        <v>72</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="P21" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" t="s">
-        <v>5</v>
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
       <c r="D23" t="s">
         <v>4</v>
       </c>
       <c r="E23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
         <v>59</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N24" t="s">
         <v>47</v>
       </c>
-      <c r="P23">
+      <c r="P24">
         <v>1</v>
       </c>
-      <c r="Q23">
+      <c r="Q24">
         <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>76</v>
-      </c>
-      <c r="N24" t="s">
-        <v>48</v>
-      </c>
-      <c r="P24">
-        <v>2</v>
-      </c>
-      <c r="Q24">
-        <v>3</v>
       </c>
     </row>
     <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P25">
+        <v>2</v>
+      </c>
+      <c r="Q25">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
+        <v>77</v>
+      </c>
+      <c r="N26" t="s">
+        <v>49</v>
+      </c>
+      <c r="P26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
         <v>75</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>62</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H27" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>4</v>
-      </c>
-      <c r="E27" t="s">
-        <v>5</v>
-      </c>
-      <c r="N27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>10</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
       </c>
+      <c r="N28" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>82</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>81</v>
-      </c>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>10</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>185</v>
+        <v>85</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
+        <v>185</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
         <v>186</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>182</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>2</v>
       </c>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
         <v>183</v>
       </c>
-      <c r="E38" s="1"/>
-      <c r="H38" t="s">
+      <c r="E39" s="1"/>
+      <c r="H39" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E39" s="1"/>
-    </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>15</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>16</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>194</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
         <v>197</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H51" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>188</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>192</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
         <v>23</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>24</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E62" t="s">
         <v>59</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G62" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
         <v>213</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>2</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" t="s">
         <v>7</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F71" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>90</v>
-      </c>
-      <c r="E71" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E72" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>198</v>
+        <v>80</v>
+      </c>
+      <c r="E73" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>200</v>
-      </c>
-      <c r="G75" t="s">
-        <v>87</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+      <c r="G76" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>205</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>206</v>
-      </c>
-      <c r="E81" s="2"/>
+        <v>205</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>207</v>
-      </c>
-      <c r="E82" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="E82" s="3"/>
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
-        <v>208</v>
-      </c>
-      <c r="E83" s="2"/>
+        <v>207</v>
+      </c>
+      <c r="E83" s="3"/>
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D84" t="s">
-        <v>30</v>
-      </c>
-      <c r="E84" t="s">
-        <v>5</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="E84" s="3"/>
     </row>
     <row r="85" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E85" t="s">
         <v>5</v>
@@ -1670,794 +1670,802 @@
     </row>
     <row r="86" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
-        <v>209</v>
+        <v>31</v>
       </c>
       <c r="E86" t="s">
-        <v>216</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
-        <v>210</v>
+        <v>209</v>
+      </c>
+      <c r="E87" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="88" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D89" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="90" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D90" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="91" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D91" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
         <v>222</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E92" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="93" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C93" t="s">
+    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
         <v>125</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>2</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E94" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D94" t="s">
-        <v>86</v>
-      </c>
-      <c r="E94" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="95" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D95" t="s">
-        <v>32</v>
+        <v>86</v>
+      </c>
+      <c r="E95" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D96" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
         <v>34</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F98" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
+    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
         <v>217</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>2</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D100" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
-        <v>192</v>
+        <v>90</v>
       </c>
     </row>
     <row r="103" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
     </row>
     <row r="104" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="105" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D105" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="106" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C107" t="s">
+    <row r="108" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
         <v>35</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D108" t="s">
         <v>31</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E108" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D108" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="111" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
+    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
         <v>36</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D113" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D113" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="114" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="115" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C116" t="s">
+    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
         <v>40</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D117" t="s">
         <v>30</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E117" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D117" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="118" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="120" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C121" t="s">
+    <row r="122" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
         <v>44</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D122" t="s">
         <v>2</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E122" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D122" t="s">
-        <v>96</v>
-      </c>
-      <c r="E122" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="123" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
-        <v>24</v>
+        <v>96</v>
+      </c>
+      <c r="E123" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="124" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="125" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="126" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
-        <v>224</v>
+        <v>45</v>
       </c>
     </row>
     <row r="127" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="128" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C130" t="s">
+    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
         <v>43</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D131" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D131" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="132" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="133" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="134" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D134" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C136" t="s">
+    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
         <v>109</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D137" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D137" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="138" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="139" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="140" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="141" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="142" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="143" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C145" t="s">
+    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C146" t="s">
         <v>115</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D146" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D146" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="147" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
     </row>
     <row r="148" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
     </row>
     <row r="149" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
     </row>
     <row r="150" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C152" t="s">
+    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C153" t="s">
         <v>136</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D153" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D153" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="154" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="155" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="156" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="157" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C159" t="s">
+    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C160" t="s">
         <v>137</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D160" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D160" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="161" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D161" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
     </row>
     <row r="162" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="163" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="164" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D165" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C166" t="s">
+    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C167" t="s">
         <v>149</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D167" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D167" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="168" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
     </row>
     <row r="169" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D169" t="s">
-        <v>152</v>
+        <v>16</v>
       </c>
     </row>
     <row r="170" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D170" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="171" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="172" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D172" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="173" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D173" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="174" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D174" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D175" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C176" t="s">
+    <row r="177" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
         <v>150</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D177" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="177" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D177" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="178" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D178" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="179" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D179" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
     </row>
     <row r="180" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
-        <v>229</v>
+        <v>130</v>
       </c>
     </row>
     <row r="181" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="182" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D182" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="183" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D183" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="184" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D184" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="185" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C185" t="s">
+    <row r="186" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C186" t="s">
         <v>138</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D186" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="186" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D186" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="187" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="188" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="189" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D189" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="190" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D190" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="191" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C191" t="s">
+    <row r="192" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C192" t="s">
         <v>139</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D192" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="192" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D192" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="193" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D193" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="194" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D194" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
     </row>
     <row r="195" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="196" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D196" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="197" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D197" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="198" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C198" t="s">
+    <row r="199" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C199" t="s">
         <v>230</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D199" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="199" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D199" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="200" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="201" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="202" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D202" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="203" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C203" t="s">
+    <row r="204" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C204" t="s">
         <v>231</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D204" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="204" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D204" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="205" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D205" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="206" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D206" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
     </row>
     <row r="207" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D207" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="208" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D208" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D209" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C210" t="s">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C211" t="s">
         <v>159</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D211" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D211" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D212" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D213" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D214" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D216" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C217" t="s">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C218" t="s">
         <v>160</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D218" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D218" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D219" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D220" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D221" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D222" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B223" t="s">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
         <v>105</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C224" t="s">
         <v>106</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D224" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D224" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="225" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D225" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="226" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D226" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="227" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C227" t="s">
+    <row r="228" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C228" t="s">
         <v>121</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D228" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="228" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D228" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="229" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D229" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="230" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D230" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="231" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D231" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="232" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D232" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="233" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C233" t="s">
+    <row r="234" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C234" t="s">
         <v>122</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D234" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="234" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D234" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="235" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D235" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="236" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D236" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="237" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D237" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="238" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D238" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="239" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C239" t="s">
+    <row r="240" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C240" t="s">
         <v>147</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D240" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="240" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D240" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D241" t="s">
-        <v>177</v>
+        <v>107</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D242" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D243" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D244" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D245" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B246" t="s">
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
         <v>181</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="E81:E84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Change in some user interface
as per summary
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.alpha.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.alpha.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="236">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -137,12 +137,6 @@
     <t>convert_unit_id_2</t>
   </si>
   <si>
-    <t>MASTER TAG</t>
-  </si>
-  <si>
-    <t>tags_name</t>
-  </si>
-  <si>
     <t>purchase_datetime</t>
   </si>
   <si>
@@ -296,15 +290,9 @@
     <t>unit_description</t>
   </si>
   <si>
-    <t>tags_desctiption</t>
-  </si>
-  <si>
     <t>unit_active</t>
   </si>
   <si>
-    <t>tags_active</t>
-  </si>
-  <si>
     <t>purchase_invoice</t>
   </si>
   <si>
@@ -717,6 +705,24 @@
   </si>
   <si>
     <t>user_password</t>
+  </si>
+  <si>
+    <t>MASTER CATEGORY</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>category_name</t>
+  </si>
+  <si>
+    <t>category_desctiption</t>
+  </si>
+  <si>
+    <t>category_active</t>
+  </si>
+  <si>
+    <t>branch_active</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q247"/>
+  <dimension ref="B1:Q252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1088,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
@@ -1098,13 +1104,13 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1115,915 +1121,903 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" t="s">
         <v>59</v>
-      </c>
-      <c r="G16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>233</v>
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>3</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" t="s">
-        <v>72</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="P22" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" t="s">
-        <v>5</v>
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" t="s">
+        <v>70</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="P23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
-      </c>
-      <c r="N24" t="s">
-        <v>47</v>
-      </c>
-      <c r="P24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>57</v>
+      </c>
+      <c r="N26" t="s">
+        <v>45</v>
+      </c>
+      <c r="P26">
         <v>1</v>
       </c>
-      <c r="Q24">
+      <c r="Q26">
         <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>76</v>
-      </c>
-      <c r="N25" t="s">
-        <v>48</v>
-      </c>
-      <c r="P25">
-        <v>2</v>
-      </c>
-      <c r="Q25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>77</v>
-      </c>
-      <c r="N26" t="s">
-        <v>49</v>
-      </c>
-      <c r="P26">
-        <v>3</v>
       </c>
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
+        <v>74</v>
+      </c>
+      <c r="N27" t="s">
+        <v>46</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
+      <c r="Q27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
         <v>75</v>
       </c>
-      <c r="F27" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" t="s">
-        <v>5</v>
-      </c>
       <c r="N28" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="P28">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
+      </c>
+      <c r="F29" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="N31" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>84</v>
-      </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>186</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>187</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="E37" s="1"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>182</v>
-      </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>182</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="H39" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" t="s">
-        <v>59</v>
-      </c>
+      <c r="E42" s="1"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>178</v>
+      </c>
       <c r="D43" t="s">
-        <v>17</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E43" s="1"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>18</v>
+        <v>179</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="H44" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
-        <v>19</v>
-      </c>
+      <c r="E45" s="1"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
-        <v>20</v>
+      <c r="B46" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
       <c r="D47" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="E47" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>197</v>
-      </c>
-      <c r="H51" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>193</v>
+      </c>
+      <c r="H56" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>184</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>188</v>
       </c>
-      <c r="D53" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
         <v>23</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D67" t="s">
         <v>24</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G67" t="s">
         <v>59</v>
-      </c>
-      <c r="G62" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D65" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D67" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>79</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>66</v>
+      <c r="D70" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>213</v>
-      </c>
       <c r="D71" t="s">
-        <v>2</v>
-      </c>
-      <c r="E71" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>90</v>
-      </c>
-      <c r="E72" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>80</v>
-      </c>
-      <c r="E73" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>198</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>199</v>
+      <c r="B75" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>209</v>
+      </c>
       <c r="D76" t="s">
-        <v>200</v>
-      </c>
-      <c r="G76" t="s">
-        <v>87</v>
+        <v>2</v>
+      </c>
+      <c r="E76" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>201</v>
+        <v>88</v>
+      </c>
+      <c r="E77" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>202</v>
+        <v>78</v>
+      </c>
+      <c r="E78" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="81" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>196</v>
+      </c>
+      <c r="G81" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="83" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="84" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="85" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>201</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>202</v>
+      </c>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>203</v>
+      </c>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D81" t="s">
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>30</v>
+      </c>
+      <c r="E90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>31</v>
+      </c>
+      <c r="E91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
         <v>205</v>
       </c>
-      <c r="E81" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D82" t="s">
+      <c r="E92" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
         <v>206</v>
       </c>
-      <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
+    </row>
+    <row r="94" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
         <v>207</v>
       </c>
-      <c r="E83" s="3"/>
-    </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
+    </row>
+    <row r="95" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
         <v>208</v>
       </c>
-      <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>30</v>
-      </c>
-      <c r="E85" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>31</v>
-      </c>
-      <c r="E86" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D87" t="s">
-        <v>209</v>
-      </c>
-      <c r="E87" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D88" t="s">
+    </row>
+    <row r="96" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D90" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D91" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="92" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D92" t="s">
-        <v>222</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C94" t="s">
-        <v>125</v>
-      </c>
-      <c r="D94" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="95" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D95" t="s">
-        <v>86</v>
-      </c>
-      <c r="E95" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D96" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="97" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
-        <v>34</v>
-      </c>
-      <c r="F98" t="s">
-        <v>97</v>
+        <v>218</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>121</v>
+      </c>
+      <c r="D99" t="s">
+        <v>2</v>
+      </c>
+      <c r="E99" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C100" t="s">
-        <v>217</v>
-      </c>
       <c r="D100" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="E100" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
-        <v>218</v>
+        <v>32</v>
       </c>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
-        <v>90</v>
+        <v>33</v>
       </c>
     </row>
     <row r="103" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
-        <v>219</v>
+        <v>34</v>
+      </c>
+      <c r="F103" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="105" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>213</v>
+      </c>
       <c r="D105" t="s">
-        <v>220</v>
+        <v>2</v>
+      </c>
+      <c r="E105" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
-        <v>221</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="107" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="108" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C108" t="s">
-        <v>35</v>
-      </c>
       <c r="D108" t="s">
-        <v>31</v>
-      </c>
-      <c r="E108" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>91</v>
+        <v>215</v>
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
-        <v>92</v>
+        <v>216</v>
       </c>
     </row>
     <row r="111" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
-        <v>94</v>
+        <v>217</v>
       </c>
     </row>
     <row r="113" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C113" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D113" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="E113" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="114" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="115" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C117" t="s">
-        <v>40</v>
-      </c>
-      <c r="D117" t="s">
-        <v>30</v>
-      </c>
-      <c r="E117" t="s">
-        <v>8</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="118" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>36</v>
+      </c>
       <c r="D118" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="119" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
     </row>
     <row r="120" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
     </row>
     <row r="122" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
-        <v>44</v>
+        <v>230</v>
       </c>
       <c r="D122" t="s">
-        <v>2</v>
+        <v>231</v>
       </c>
       <c r="E122" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
-        <v>96</v>
-      </c>
-      <c r="E123" t="s">
-        <v>8</v>
+        <v>232</v>
       </c>
     </row>
     <row r="124" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
-        <v>24</v>
+        <v>233</v>
       </c>
     </row>
     <row r="125" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="127" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="126" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D126" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="127" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
-        <v>224</v>
+        <v>2</v>
+      </c>
+      <c r="E127" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
-        <v>225</v>
+        <v>92</v>
+      </c>
+      <c r="E128" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
-        <v>120</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="131" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>43</v>
-      </c>
-      <c r="D131" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="132" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
-        <v>86</v>
+        <v>220</v>
       </c>
     </row>
     <row r="133" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
-        <v>119</v>
+        <v>221</v>
       </c>
     </row>
     <row r="134" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D134" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D135" t="s">
-        <v>46</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C136" t="s">
+        <v>41</v>
+      </c>
+      <c r="D136" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="137" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C137" t="s">
-        <v>109</v>
-      </c>
       <c r="D137" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="138" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="139" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
     </row>
     <row r="140" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D141" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
     </row>
     <row r="142" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C142" t="s">
+        <v>105</v>
+      </c>
       <c r="D142" t="s">
-        <v>114</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="144" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="146" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C146" t="s">
-        <v>115</v>
-      </c>
       <c r="D146" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="147" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
     </row>
     <row r="148" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="149" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D150" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="151" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C151" t="s">
+        <v>111</v>
+      </c>
       <c r="D151" t="s">
-        <v>132</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="153" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C153" t="s">
-        <v>136</v>
-      </c>
       <c r="D153" t="s">
-        <v>2</v>
+        <v>120</v>
       </c>
     </row>
     <row r="154" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
     </row>
     <row r="155" spans="3:4" x14ac:dyDescent="0.25">
@@ -2036,436 +2030,459 @@
         <v>128</v>
       </c>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D157" t="s">
-        <v>129</v>
-      </c>
-    </row>
     <row r="158" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C158" t="s">
+        <v>132</v>
+      </c>
       <c r="D158" t="s">
-        <v>168</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="160" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C160" t="s">
-        <v>137</v>
-      </c>
       <c r="D160" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="161" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D161" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
     </row>
     <row r="162" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="163" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D164" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
     </row>
     <row r="165" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C165" t="s">
+        <v>133</v>
+      </c>
       <c r="D165" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="167" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C167" t="s">
-        <v>149</v>
-      </c>
       <c r="D167" t="s">
-        <v>2</v>
+        <v>120</v>
       </c>
     </row>
     <row r="168" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
     </row>
     <row r="169" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D169" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
     </row>
     <row r="170" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D170" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D171" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
     </row>
     <row r="172" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C172" t="s">
+        <v>145</v>
+      </c>
       <c r="D172" t="s">
-        <v>154</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D173" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="174" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D174" t="s">
-        <v>156</v>
+        <v>16</v>
       </c>
     </row>
     <row r="175" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D175" t="s">
-        <v>157</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D176" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="177" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C177" t="s">
+      <c r="D177" t="s">
         <v>150</v>
-      </c>
-      <c r="D177" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="178" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D178" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
     </row>
     <row r="179" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D179" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
     </row>
     <row r="180" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="181" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D181" t="s">
-        <v>229</v>
+        <v>153</v>
       </c>
     </row>
     <row r="182" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C182" t="s">
+        <v>146</v>
+      </c>
       <c r="D182" t="s">
-        <v>226</v>
+        <v>154</v>
       </c>
     </row>
     <row r="183" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D183" t="s">
-        <v>227</v>
+        <v>84</v>
       </c>
     </row>
     <row r="184" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D184" t="s">
-        <v>228</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="185" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D185" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="186" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C186" t="s">
-        <v>138</v>
-      </c>
       <c r="D186" t="s">
-        <v>2</v>
+        <v>225</v>
       </c>
     </row>
     <row r="187" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
-        <v>140</v>
+        <v>222</v>
       </c>
     </row>
     <row r="188" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>141</v>
+        <v>223</v>
       </c>
     </row>
     <row r="189" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D189" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="190" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D190" t="s">
-        <v>143</v>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="191" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C191" t="s">
+        <v>134</v>
+      </c>
+      <c r="D191" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="192" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C192" t="s">
-        <v>139</v>
-      </c>
       <c r="D192" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="193" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D193" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
     </row>
     <row r="194" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D194" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
     </row>
     <row r="195" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="196" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D196" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="197" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C197" t="s">
+        <v>135</v>
+      </c>
       <c r="D197" t="s">
-        <v>146</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="198" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D198" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="199" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C199" t="s">
-        <v>230</v>
-      </c>
       <c r="D199" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
     </row>
     <row r="200" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="201" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="202" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D202" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="204" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C204" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D204" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D205" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
     </row>
     <row r="206" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D206" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
     </row>
     <row r="207" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D207" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="208" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D208" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="209" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C209" t="s">
+        <v>227</v>
+      </c>
       <c r="D209" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C211" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="210" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D210" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="211" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D211" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="212" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D212" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="213" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D213" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="214" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D214" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="216" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C216" t="s">
+        <v>155</v>
+      </c>
+      <c r="D216" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D217" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="218" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D218" t="s">
         <v>159</v>
       </c>
-      <c r="D211" t="s">
+    </row>
+    <row r="219" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D219" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="220" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D220" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="221" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D221" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="223" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C223" t="s">
+        <v>156</v>
+      </c>
+      <c r="D223" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="224" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D224" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D225" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D226" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D227" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
+        <v>101</v>
+      </c>
+      <c r="C229" t="s">
+        <v>102</v>
+      </c>
+      <c r="D229" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D212" t="s">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D230" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D231" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C233" t="s">
+        <v>117</v>
+      </c>
+      <c r="D233" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D234" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D235" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D236" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D213" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D214" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D215" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D216" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C218" t="s">
-        <v>160</v>
-      </c>
-      <c r="D218" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D219" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D220" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D221" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D222" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B224" t="s">
-        <v>105</v>
-      </c>
-      <c r="C224" t="s">
-        <v>106</v>
-      </c>
-      <c r="D224" t="s">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D237" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C239" t="s">
+        <v>118</v>
+      </c>
+      <c r="D239" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D225" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="226" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D226" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="228" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C228" t="s">
-        <v>121</v>
-      </c>
-      <c r="D228" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="229" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D229" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="230" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D230" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="231" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D231" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="232" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D232" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="234" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C234" t="s">
-        <v>122</v>
-      </c>
-      <c r="D234" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="235" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D235" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="236" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D236" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="237" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D237" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="238" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D238" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="240" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C240" t="s">
-        <v>147</v>
-      </c>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D240" t="s">
-        <v>2</v>
+        <v>168</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D241" t="s">
-        <v>107</v>
+        <v>169</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D242" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D243" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D244" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C245" t="s">
+        <v>143</v>
+      </c>
       <c r="D245" t="s">
-        <v>180</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D246" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B247" t="s">
-        <v>181</v>
+      <c r="D247" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D248" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D249" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D250" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B252" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E81:E84"/>
+    <mergeCell ref="E86:E89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2484,21 +2501,21 @@
   <sheetData>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>52</v>
-      </c>
-      <c r="F9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2512,7 +2529,7 @@
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E11">
         <v>0</v>

</xml_diff>